<commit_message>
Balaceamento dos niveis dos monstros
</commit_message>
<xml_diff>
--- a/estrutura/Bestiario.xlsx
+++ b/estrutura/Bestiario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pasta Dev\Masmorra_fim\estrutura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUPORTE 03\Desktop\EU\Eu (Carlos)\Cod_Dev\Masmorra_fim\estrutura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1810CB8C-6E11-4CA8-B3C9-E84AE5DA7712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCFDD16-354D-4ED0-8193-ECBAF47B8EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-60" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestiario" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
   <si>
     <t>nome</t>
   </si>
@@ -321,13 +321,46 @@
   </si>
   <si>
     <t>80 - 90</t>
+  </si>
+  <si>
+    <t>Clone Corrompido</t>
+  </si>
+  <si>
+    <t>Player(classe)</t>
+  </si>
+  <si>
+    <t>Player + 5</t>
+  </si>
+  <si>
+    <t>Player + 2</t>
+  </si>
+  <si>
+    <t>player + 1</t>
+  </si>
+  <si>
+    <t>Player(habilidade)</t>
+  </si>
+  <si>
+    <t>Kharath, o Lamento Encarnado</t>
+  </si>
+  <si>
+    <t>Corte Maligno</t>
+  </si>
+  <si>
+    <t>Teia Sombria</t>
+  </si>
+  <si>
+    <t>Entidade</t>
+  </si>
+  <si>
+    <t>Obliterar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,8 +524,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +585,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F497D"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -625,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -728,6 +774,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -746,7 +795,19 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1060,39 +1121,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="46.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
@@ -1100,7 +1163,7 @@
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
     </row>
-    <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1201,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
     </row>
-    <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1176,7 +1239,7 @@
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1214,36 +1277,36 @@
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
     </row>
-    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="30">
-        <v>45</v>
-      </c>
-      <c r="D5" s="30">
-        <v>33</v>
-      </c>
-      <c r="E5" s="30">
-        <v>45</v>
-      </c>
-      <c r="F5" s="30">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3</v>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="I5" s="2">
-        <v>60</v>
-      </c>
-      <c r="J5" s="4">
-        <v>3</v>
+        <v>100</v>
+      </c>
+      <c r="J5" s="43">
+        <v>2</v>
       </c>
       <c r="L5" s="16"/>
       <c r="M5" s="16"/>
@@ -1252,30 +1315,30 @@
       <c r="P5" s="16"/>
       <c r="Q5" s="17"/>
     </row>
-    <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="30">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D6" s="30">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E6" s="30">
         <v>45</v>
       </c>
       <c r="F6" s="30">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>42</v>
+      <c r="H6" s="2">
+        <v>3</v>
       </c>
       <c r="I6" s="2">
         <v>60</v>
@@ -1290,30 +1353,30 @@
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
     </row>
-    <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D7" s="30">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="30">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F7" s="30">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2">
         <v>60</v>
@@ -1322,62 +1385,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="30">
+        <v>95</v>
+      </c>
+      <c r="D8" s="30">
+        <v>50</v>
+      </c>
+      <c r="E8" s="30">
+        <v>50</v>
+      </c>
+      <c r="F8" s="30">
+        <v>50</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="2">
+        <v>60</v>
+      </c>
+      <c r="J8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="30">
-        <v>70</v>
-      </c>
-      <c r="D8" s="30">
-        <v>39</v>
-      </c>
-      <c r="E8" s="30">
-        <v>20</v>
-      </c>
-      <c r="F8" s="30">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2">
-        <v>90</v>
-      </c>
-      <c r="J8" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="30">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D9" s="30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E9" s="30">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F9" s="30">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="2">
         <v>90</v>
@@ -1386,30 +1449,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C10" s="30">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D10" s="30">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E10" s="30">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F10" s="30">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
       </c>
       <c r="I10" s="2">
         <v>90</v>
@@ -1419,42 +1482,42 @@
       </c>
       <c r="S10" s="16"/>
     </row>
-    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="30">
         <v>120</v>
       </c>
       <c r="D11" s="30">
-        <v>45</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="E11" s="30">
+        <v>40</v>
       </c>
       <c r="F11" s="30">
         <v>80</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I11" s="2">
-        <v>290</v>
+        <v>90</v>
       </c>
       <c r="J11" s="5">
         <v>4</v>
       </c>
       <c r="S11" s="16"/>
     </row>
-    <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>26</v>
@@ -1463,7 +1526,7 @@
         <v>120</v>
       </c>
       <c r="D12" s="30">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>46</v>
@@ -1485,114 +1548,114 @@
       </c>
       <c r="S12" s="17"/>
     </row>
-    <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="30">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D13" s="30">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="30">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2">
+        <v>290</v>
+      </c>
+      <c r="J13" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="30">
+        <v>80</v>
+      </c>
+      <c r="D14" s="30">
+        <v>55</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="30">
+        <v>55</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <v>5</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I14" s="2">
         <v>120</v>
-      </c>
-      <c r="J13" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="30">
-        <v>100</v>
-      </c>
-      <c r="D14" s="30">
-        <v>50</v>
-      </c>
-      <c r="E14" s="30">
-        <v>100</v>
-      </c>
-      <c r="F14" s="30">
-        <v>70</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="2">
-        <v>8</v>
-      </c>
-      <c r="I14" s="2">
-        <v>320</v>
       </c>
       <c r="J14" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>26</v>
+        <v>74</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="30">
+        <v>140</v>
+      </c>
+      <c r="D15" s="30">
+        <v>60</v>
+      </c>
+      <c r="E15" s="30">
         <v>100</v>
       </c>
-      <c r="D15" s="30">
-        <v>44</v>
-      </c>
-      <c r="E15" s="30">
-        <v>30</v>
-      </c>
       <c r="F15" s="30">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I15" s="2">
-        <v>120</v>
+        <v>320</v>
       </c>
       <c r="J15" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C16" s="30">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D16" s="30">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E16" s="30">
         <v>30</v>
@@ -1601,7 +1664,7 @@
         <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="H16" s="2">
         <v>7</v>
@@ -1613,88 +1676,88 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="30">
+        <v>130</v>
+      </c>
+      <c r="D17" s="30">
+        <v>60</v>
+      </c>
+      <c r="E17" s="30">
         <v>30</v>
       </c>
-      <c r="C17" s="30">
-        <v>120</v>
-      </c>
-      <c r="D17" s="30">
-        <v>57</v>
-      </c>
-      <c r="E17" s="30">
+      <c r="F17" s="30">
         <v>80</v>
       </c>
-      <c r="F17" s="30">
-        <v>70</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="H17" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I17" s="2">
         <v>120</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="30">
+        <v>140</v>
+      </c>
+      <c r="D18" s="30">
+        <v>66</v>
+      </c>
+      <c r="E18" s="30">
+        <v>80</v>
+      </c>
+      <c r="F18" s="30">
+        <v>70</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2">
+        <v>120</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="30">
-        <v>80</v>
-      </c>
-      <c r="D18" s="30">
-        <v>45</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="30">
-        <v>66</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="2">
-        <v>7</v>
-      </c>
-      <c r="I18" s="2">
-        <v>150</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="C19" s="30">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D19" s="30">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="30">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>46</v>
@@ -1709,59 +1772,59 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="30">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D20" s="30">
-        <v>60</v>
-      </c>
-      <c r="E20" s="30">
-        <v>80</v>
+        <v>65</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="F20" s="30">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H20" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I20" s="2">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="30">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D21" s="30">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E21" s="30">
         <v>80</v>
       </c>
       <c r="F21" s="30">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H21" s="2">
         <v>9</v>
@@ -1773,71 +1836,71 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="30">
+        <v>144</v>
+      </c>
+      <c r="D22" s="30">
+        <v>70</v>
+      </c>
+      <c r="E22" s="30">
+        <v>80</v>
+      </c>
+      <c r="F22" s="30">
+        <v>70</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="2">
+        <v>9</v>
+      </c>
+      <c r="I22" s="2">
+        <v>350</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="30">
-        <v>120</v>
-      </c>
-      <c r="D22" s="30">
-        <v>57</v>
-      </c>
-      <c r="E22" s="30">
+      <c r="C23" s="30">
+        <v>180</v>
+      </c>
+      <c r="D23" s="30">
+        <v>75</v>
+      </c>
+      <c r="E23" s="30">
         <v>90</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F23" s="30">
         <v>80</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H22" s="2">
-        <v>10</v>
-      </c>
-      <c r="I22" s="2">
-        <v>400</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="30">
-        <v>150</v>
-      </c>
-      <c r="D23" s="30">
-        <v>60</v>
-      </c>
-      <c r="E23" s="30">
-        <v>80</v>
-      </c>
-      <c r="F23" s="30">
-        <v>70</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="H23" s="2">
         <v>10</v>
       </c>
       <c r="I23" s="2">
-        <v>300</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>61</v>
       </c>
@@ -1845,74 +1908,74 @@
         <v>31</v>
       </c>
       <c r="C24" s="30">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="D24" s="30">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E24" s="30">
         <v>80</v>
       </c>
       <c r="F24" s="30">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="H24" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I24" s="2">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="C25" s="30">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="D25" s="30">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E25" s="30">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F25" s="30">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="H25" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I25" s="2">
         <v>200</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="C26" s="30">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D26" s="30">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E26" s="30">
         <v>90</v>
@@ -1921,106 +1984,106 @@
         <v>80</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H26" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I26" s="2">
         <v>200</v>
       </c>
-      <c r="J26" s="33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="J26" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="30">
+        <v>210</v>
+      </c>
+      <c r="D27" s="30">
         <v>80</v>
       </c>
-      <c r="C27" s="30">
-        <v>40</v>
-      </c>
-      <c r="D27" s="30">
-        <v>30</v>
-      </c>
       <c r="E27" s="30">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F27" s="30">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="H27" s="2">
+        <v>11</v>
       </c>
       <c r="I27" s="2">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="J27" s="33">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="30">
+        <v>40</v>
+      </c>
+      <c r="D28" s="30">
+        <v>10</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="30">
+        <v>60</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="2">
+        <v>50</v>
+      </c>
+      <c r="J28" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="30">
-        <v>99</v>
-      </c>
-      <c r="D28" s="30">
-        <v>80</v>
-      </c>
-      <c r="E28" s="30">
-        <v>0</v>
-      </c>
-      <c r="F28" s="30">
-        <v>70</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="2">
-        <v>9</v>
-      </c>
-      <c r="I28" s="2">
-        <v>200</v>
-      </c>
-      <c r="J28" s="34">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="30">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D29" s="30">
-        <v>85</v>
-      </c>
-      <c r="E29" s="30">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="F29" s="30">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H29" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I29" s="2">
         <v>200</v>
@@ -2029,30 +2092,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="30">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D30" s="30">
-        <v>90</v>
-      </c>
-      <c r="E30" s="30">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="F30" s="30">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H30" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I30" s="2">
         <v>200</v>
@@ -2061,30 +2124,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>27</v>
+        <v>84</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C31" s="30">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="D31" s="30">
+        <v>90</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="30">
         <v>100</v>
-      </c>
-      <c r="E31" s="30">
-        <v>70</v>
-      </c>
-      <c r="F31" s="30">
-        <v>70</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H31" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I31" s="2">
         <v>200</v>
@@ -2093,94 +2156,94 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="30">
-        <v>230</v>
+        <v>160</v>
       </c>
       <c r="D32" s="30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E32" s="30">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F32" s="30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="H32" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I32" s="2">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="J32" s="34">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>26</v>
+        <v>86</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C33" s="30">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="D33" s="30">
+        <v>100</v>
+      </c>
+      <c r="E33" s="30">
         <v>90</v>
       </c>
-      <c r="E33" s="30">
-        <v>80</v>
-      </c>
       <c r="F33" s="30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H33" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I33" s="2">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="J33" s="34">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>27</v>
+        <v>88</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C34" s="30">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="D34" s="30">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E34" s="30">
         <v>80</v>
       </c>
       <c r="F34" s="30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H34" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I34" s="2">
         <v>550</v>
@@ -2189,37 +2252,198 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="G35" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="30">
+        <v>225</v>
+      </c>
+      <c r="D35" s="30">
+        <v>110</v>
+      </c>
+      <c r="E35" s="30">
+        <v>80</v>
+      </c>
+      <c r="F35" s="30">
+        <v>100</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="2">
+        <v>13</v>
       </c>
       <c r="I35" s="2">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="J35" s="34">
         <v>9</v>
       </c>
+    </row>
+    <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="2">
+        <v>500</v>
+      </c>
+      <c r="J36" s="34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2">
+        <v>320</v>
+      </c>
+      <c r="D37" s="2">
+        <v>110</v>
+      </c>
+      <c r="E37" s="2">
+        <v>90</v>
+      </c>
+      <c r="F37" s="2">
+        <v>110</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" s="2">
+        <v>20</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5000</v>
+      </c>
+      <c r="J37" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="2">
+        <v>310</v>
+      </c>
+      <c r="D38" s="2">
+        <v>115</v>
+      </c>
+      <c r="E38" s="2">
+        <v>90</v>
+      </c>
+      <c r="F38" s="2">
+        <v>115</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H38" s="2">
+        <v>20</v>
+      </c>
+      <c r="I38" s="2">
+        <v>500</v>
+      </c>
+      <c r="J38" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="30">
+        <v>400</v>
+      </c>
+      <c r="D39" s="30">
+        <v>150</v>
+      </c>
+      <c r="E39" s="30">
+        <v>500</v>
+      </c>
+      <c r="F39" s="30">
+        <v>130</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="2">
+        <v>50</v>
+      </c>
+      <c r="I39" s="2">
+        <v>9000</v>
+      </c>
+      <c r="J39" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="46">
+        <v>500</v>
+      </c>
+      <c r="D40" s="46">
+        <v>200</v>
+      </c>
+      <c r="E40" s="46">
+        <v>500</v>
+      </c>
+      <c r="F40" s="46">
+        <v>190</v>
+      </c>
+      <c r="G40" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="47">
+        <v>100</v>
+      </c>
+      <c r="I40" s="47">
+        <v>9000</v>
+      </c>
+      <c r="J40" s="1">
+        <v>10</v>
+      </c>
+      <c r="L40" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2234,27 +2458,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDC89AD-77BA-4F5D-9C76-DFABC45F5782}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
-    </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2274,7 +2498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>27</v>
       </c>
@@ -2294,7 +2518,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>26</v>
       </c>
@@ -2314,7 +2538,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>52</v>
       </c>
@@ -2334,7 +2558,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>31</v>
       </c>
@@ -2354,8 +2578,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="28" t="s">
@@ -2374,7 +2598,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M9" s="29"/>
     </row>
   </sheetData>

</xml_diff>